<commit_message>
replace old annotation with annotation of improved bins
</commit_message>
<xml_diff>
--- a/redundant_bins_ANI.0.9_COV.0.7.xlsx
+++ b/redundant_bins_ANI.0.9_COV.0.7.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>Comparison</t>
   </si>
@@ -264,36 +264,6 @@
     <t>Limnohabitans sp. bin L4</t>
   </si>
   <si>
-    <t>Limnohabitans sp. bin L8 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L5 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L6 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L7 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L3 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L1 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Unclassified Betaproteobacteria bin B4 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L2 (reanalysis)</t>
-  </si>
-  <si>
-    <t>Limnohabitans sp. bin L4 (reanalysis)</t>
-  </si>
-  <si>
-    <t>new_AP_ID</t>
-  </si>
-  <si>
     <t>B72-73_Su13.BD.MM15.SN.C_rebin5-6_refined1</t>
   </si>
   <si>
@@ -310,6 +280,33 @@
   </si>
   <si>
     <t>Limnohabitans sp. bin L03</t>
+  </si>
+  <si>
+    <t>new_GOLD_ID</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L8r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L5r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L6r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L7r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L3r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L1r</t>
+  </si>
+  <si>
+    <t>Unclassified Betaproteobacteria bin B4r</t>
+  </si>
+  <si>
+    <t>Limnohabitans sp. bin L2r</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,13 +1803,13 @@
         <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
         <v>68</v>
       </c>
       <c r="J18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -1828,8 +1825,11 @@
       <c r="G19" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H19">
+        <v>2757320395</v>
+      </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J19">
         <v>665874</v>
@@ -1848,8 +1848,11 @@
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="H20">
+        <v>2757320396</v>
+      </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J20">
         <v>665874</v>
@@ -1868,8 +1871,11 @@
       <c r="G21" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="H21">
+        <v>2757320397</v>
+      </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="J21">
         <v>665874</v>
@@ -1888,8 +1894,11 @@
       <c r="G22" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H22">
+        <v>2757320398</v>
+      </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="J22">
         <v>665874</v>
@@ -1906,10 +1915,13 @@
         <v>74</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="H23">
+        <v>2757320399</v>
       </c>
       <c r="I23" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="J23">
         <v>665874</v>
@@ -1926,10 +1938,13 @@
         <v>75</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="H24">
+        <v>2757320400</v>
       </c>
       <c r="I24" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="J24">
         <v>665874</v>
@@ -1948,8 +1963,11 @@
       <c r="G25" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="H25">
+        <v>2757320401</v>
+      </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J25">
         <v>665874</v>
@@ -1968,8 +1986,11 @@
       <c r="G26" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H26">
+        <v>2757320402</v>
+      </c>
       <c r="I26" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J26">
         <v>665874</v>
@@ -1988,8 +2009,11 @@
       <c r="G27" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="H27">
+        <v>2757320405</v>
+      </c>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="J27">
         <v>28216</v>
@@ -2008,8 +2032,11 @@
       <c r="G28" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H28">
+        <v>2757320403</v>
+      </c>
       <c r="I28" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="J28">
         <v>665874</v>
@@ -2028,8 +2055,11 @@
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H29">
+        <v>2757320404</v>
+      </c>
       <c r="I29" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="J29">
         <v>665874</v>
@@ -2047,12 +2077,6 @@
       </c>
       <c r="G30" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="I30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J30">
-        <v>665874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove part of old binning files
</commit_message>
<xml_diff>
--- a/redundant_bins_ANI.0.9_COV.0.7.xlsx
+++ b/redundant_bins_ANI.0.9_COV.0.7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="redundant_bins_ANI.0.9_COV.0.7" sheetId="1" r:id="rId1"/>
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>